<commit_message>
rapor eşleştirme refactor edildi
</commit_message>
<xml_diff>
--- a/sorular.xlsx
+++ b/sorular.xlsx
@@ -397,52 +397,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
-    <row r="1" xml:space="preserve">
+    <row r="1">
       <c r="A1" t="str">
+        <v>SORULAR</v>
+      </c>
+      <c r="B1" t="str">
+        <v>GİTMESİ GEREKEN RAPOR</v>
+      </c>
+      <c r="C1" t="str">
+        <v>GİTTİĞİ RAPOR</v>
+      </c>
+      <c r="D1" t="str">
+        <v>EŞLEŞTİ Mİ?</v>
+      </c>
+      <c r="E1" t="str">
+        <v>CEVAP</v>
+      </c>
+    </row>
+    <row r="2" xml:space="preserve">
+      <c r="A2" t="str">
         <v>Hangi bankada bugün en yüksek POS girişi gerçekleşti?</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B2" t="str">
         <v>Günlük POS İşlemleri ve Banka Bazlı Toplamlar</v>
       </c>
-      <c r="C1" t="str" xml:space="preserve">
+      <c r="C2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     📁 Günlük POS İşlemleri ve Banka Bazlı Toplamlar
           </v>
       </c>
-      <c r="D1" t="str">
+      <c r="D2" t="str">
         <v>EVET</v>
       </c>
-      <c r="E1" t="str">
-        <v>Bugün en yüksek POS girişi olan banka VAKIFBANK POS HESABI, 1,394,500.07 TL ile öne çıkıyor.</v>
+      <c r="E2" t="str">
+        <v>Bugün en yüksek POS girişi olan banka Ziraat Bankası, toplam girişi 590,040.30 TL.</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
         <v>Günlük bazda hangi bankada giriş-çıkış farkı en yüksek?</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>Günlük POS İşlemleri ve Banka Bazlı Toplamlar</v>
       </c>
-      <c r="C2" t="str" xml:space="preserve">
+      <c r="C3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    📁 Günlük Kasa ve Banka Ozet Raporu
+                    📁 Günlük POS İşlemleri ve Banka Bazlı Toplamlar
           </v>
       </c>
-      <c r="D2" t="str">
-        <v>HAYIR</v>
-      </c>
-      <c r="E2" t="str">
-        <v>📊 No results found for your criteria.</v>
+      <c r="D3" t="str">
+        <v>EVET</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Bugün bankalara göre en yüksek günlük giriş-çıkış farkı (net) AKBANK POS HS. ile -4,276,583.43 TL olarak kaydedilmiştir.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
çıktıyı farklı bir sayfa üzerine kayıt işlemi eklendi
</commit_message>
<xml_diff>
--- a/sorular.xlsx
+++ b/sorular.xlsx
@@ -1,41 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tahir\OneDrive\Masaüstü\Klasörler\Sirius\Bossai\BossAi-Otomasyon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12165"/>
+  </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOT_CEVAPLAR" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+  <si>
+    <t>SORULAR</t>
+  </si>
+  <si>
+    <t>GİTMESİ GEREKEN RAPOR</t>
+  </si>
+  <si>
+    <t>GİTTİĞİ RAPOR</t>
+  </si>
+  <si>
+    <t>EŞLEŞTİ Mİ?</t>
+  </si>
+  <si>
+    <t>CEVAP</t>
+  </si>
+  <si>
+    <t>Hangi bankada bugün en yüksek POS girişi gerçekleşti?</t>
+  </si>
+  <si>
+    <t>Günlük POS İşlemleri ve Banka Bazlı Toplamlar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                    📁 Günlük POS İşlemleri ve Banka Bazlı Toplamlar
+          </t>
+  </si>
+  <si>
+    <t>EVET</t>
+  </si>
+  <si>
+    <t>Günlük bazda hangi bankada giriş-çıkış farkı en yüksek?</t>
+  </si>
+  <si>
+    <t>Bugün en yüksek POS girişi Ziraat Bankası'ndan, toplam 614,790.30 TL olarak gerçekleşmiştir.</t>
+  </si>
+  <si>
+    <t>Bugünkü banka bazlı girişler ve çıkışlar farkı en yüksek banka "AKBANK POS HS." olup, fark tutarı -4,276,583.43 TL'dir.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +101,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,70 +433,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.625" customWidth="1"/>
+    <col min="2" max="2" width="57.875" customWidth="1"/>
+    <col min="3" max="3" width="34.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.375" customWidth="1"/>
+    <col min="3" max="3" width="37.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>SORULAR</v>
-      </c>
-      <c r="B1" t="str">
-        <v>GİTMESİ GEREKEN RAPOR</v>
-      </c>
-      <c r="C1" t="str">
-        <v>GİTTİĞİ RAPOR</v>
-      </c>
-      <c r="D1" t="str">
-        <v>EŞLEŞTİ Mİ?</v>
-      </c>
-      <c r="E1" t="str">
-        <v>CEVAP</v>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>Hangi bankada bugün en yüksek POS girişi gerçekleşti?</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Günlük POS İşlemleri ve Banka Bazlı Toplamlar</v>
-      </c>
-      <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    📁 Günlük POS İşlemleri ve Banka Bazlı Toplamlar
-          </v>
-      </c>
-      <c r="D2" t="str">
-        <v>EVET</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Bugün en yüksek POS girişi olan banka Ziraat Bankası, toplam girişi 590,040.30 TL.</v>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Günlük bazda hangi bankada giriş-çıkış farkı en yüksek?</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Günlük POS İşlemleri ve Banka Bazlı Toplamlar</v>
-      </c>
-      <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    📁 Günlük POS İşlemleri ve Banka Bazlı Toplamlar
-          </v>
-      </c>
-      <c r="D3" t="str">
-        <v>EVET</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Bugün bankalara göre en yüksek günlük giriş-çıkış farkı (net) AKBANK POS HS. ile -4,276,583.43 TL olarak kaydedilmiştir.</v>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError sqref="A1:E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>